<commit_message>
Update Requirements Table Rev1.xlsx
</commit_message>
<xml_diff>
--- a/Requirements Table Rev1.xlsx
+++ b/Requirements Table Rev1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robbie\Documents\GitHub\FundamentalsPokerGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F6C03445-601B-4B10-B5EB-A587029B9FB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD06F40-4E73-4F80-BBF6-541ED35EBCA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9F63A9F9-7C5B-4B89-AA9A-0F55721D7DEB}"/>
   </bookViews>
@@ -339,15 +339,6 @@
     <t>Game::check()</t>
   </si>
   <si>
-    <t>Game::bet()</t>
-  </si>
-  <si>
-    <t>Game::call()</t>
-  </si>
-  <si>
-    <t>Game::raise()</t>
-  </si>
-  <si>
     <t>Game::fold()</t>
   </si>
   <si>
@@ -386,6 +377,18 @@
   <si>
     <t>Game::next_stage()
 Game::game_stage</t>
+  </si>
+  <si>
+    <t>Game::bet()
+Player::on_bet_value_changed()</t>
+  </si>
+  <si>
+    <t>Game::raise()
+Player::on_bet_value_changed()</t>
+  </si>
+  <si>
+    <t>Game::call()
+Player::on_bet_value_changed()</t>
   </si>
 </sst>
 </file>
@@ -599,22 +602,6 @@
   </cellStyles>
   <dxfs count="13">
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -771,25 +758,41 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -806,17 +809,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F172631C-DAD8-4B9D-83D0-9647EE7C2F7D}" name="Table1" displayName="Table1" ref="A1:H62" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="11" tableBorderDxfId="12" totalsRowBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F172631C-DAD8-4B9D-83D0-9647EE7C2F7D}" name="Table1" displayName="Table1" ref="A1:H62" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9" totalsRowBorderDxfId="8">
   <autoFilter ref="A1:H62" xr:uid="{A4B7DCE6-B54B-42E6-97CB-19C3C7468B67}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{E3041E8D-CC89-4D3F-87D8-5AD3D54ACC50}" name="REQID" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{FF69D575-8664-4A68-95AD-D9C503EA1B5B}" name="F/NF" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{029790CB-BDCF-4D3D-A5AE-9967DB685880}" name="DEALER / PLAYER" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{B507AC89-AEB8-48F0-B9C4-BE4797BDA6C2}" name="DESCRIPTION" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{94E24771-1666-4F2D-AFD6-14DD813F19EE}" name="TEST CASE" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{5614A365-D9A5-4376-B965-FF170E8D9CE7}" name="SOURCE" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{43A05868-DA2F-4DA3-B864-83A871B3B654}" name="CLASS / METHOD" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{F342773B-66B6-48D7-B0A4-0FFF15BA8D10}" name="NOTES" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{E3041E8D-CC89-4D3F-87D8-5AD3D54ACC50}" name="REQID" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{FF69D575-8664-4A68-95AD-D9C503EA1B5B}" name="F/NF" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{029790CB-BDCF-4D3D-A5AE-9967DB685880}" name="DEALER / PLAYER" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{B507AC89-AEB8-48F0-B9C4-BE4797BDA6C2}" name="DESCRIPTION" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{94E24771-1666-4F2D-AFD6-14DD813F19EE}" name="TEST CASE" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{5614A365-D9A5-4376-B965-FF170E8D9CE7}" name="SOURCE" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{43A05868-DA2F-4DA3-B864-83A871B3B654}" name="CLASS / METHOD" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{F342773B-66B6-48D7-B0A4-0FFF15BA8D10}" name="NOTES" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1130,7 +1133,7 @@
     <col min="3" max="3" width="18" style="1" customWidth="1"/>
     <col min="4" max="5" width="40.7109375" style="2" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="26.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="30.7109375" style="1" customWidth="1"/>
     <col min="8" max="8" width="20.7109375" style="1" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -1181,7 +1184,7 @@
         <v>83</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H2" s="8"/>
     </row>
@@ -1227,7 +1230,7 @@
         <v>83</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="H4" s="8"/>
     </row>
@@ -1359,7 +1362,7 @@
         <v>87</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H10" s="8"/>
     </row>
@@ -1605,7 +1608,7 @@
         <v>87</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="H21" s="8"/>
     </row>
@@ -1629,7 +1632,7 @@
         <v>87</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="H22" s="8"/>
     </row>
@@ -1701,7 +1704,7 @@
       </c>
       <c r="H25" s="8"/>
     </row>
-    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>10.050000000000001</v>
       </c>
@@ -1719,7 +1722,7 @@
         <v>87</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="H26" s="8"/>
     </row>
@@ -1767,7 +1770,7 @@
         <v>87</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="H28" s="8"/>
     </row>
@@ -1791,7 +1794,7 @@
         <v>87</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="H29" s="8"/>
     </row>
@@ -1837,7 +1840,7 @@
         <v>87</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="H31" s="8"/>
     </row>
@@ -1883,7 +1886,7 @@
         <v>87</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H33" s="8"/>
     </row>
@@ -1907,7 +1910,7 @@
         <v>87</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="H34" s="8"/>
     </row>
@@ -1995,7 +1998,7 @@
         <v>87</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="H38" s="8"/>
     </row>
@@ -2037,7 +2040,7 @@
         <v>87</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H40" s="8"/>
     </row>
@@ -2059,7 +2062,7 @@
         <v>87</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H41" s="8"/>
     </row>
@@ -2081,7 +2084,7 @@
         <v>87</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H42" s="8"/>
     </row>
@@ -2103,7 +2106,7 @@
         <v>87</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H43" s="8"/>
     </row>
@@ -2125,7 +2128,7 @@
         <v>87</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H44" s="8"/>
     </row>
@@ -2147,7 +2150,7 @@
         <v>87</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H45" s="8"/>
     </row>
@@ -2169,7 +2172,7 @@
         <v>87</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H46" s="8"/>
     </row>
@@ -2191,7 +2194,7 @@
         <v>87</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H47" s="8"/>
     </row>
@@ -2213,7 +2216,7 @@
         <v>87</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H48" s="8"/>
     </row>
@@ -2235,7 +2238,7 @@
         <v>87</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H49" s="8"/>
     </row>
@@ -2257,7 +2260,7 @@
         <v>87</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H50" s="8"/>
     </row>
@@ -2279,7 +2282,7 @@
         <v>87</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H51" s="8"/>
     </row>
@@ -2301,7 +2304,7 @@
         <v>87</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H52" s="8"/>
     </row>
@@ -2323,7 +2326,7 @@
         <v>87</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H53" s="8"/>
     </row>
@@ -2345,7 +2348,7 @@
         <v>87</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H54" s="8"/>
     </row>
@@ -2367,7 +2370,7 @@
         <v>87</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H55" s="8"/>
     </row>
@@ -2389,7 +2392,7 @@
         <v>87</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H56" s="8"/>
     </row>
@@ -2411,7 +2414,7 @@
         <v>87</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H57" s="8"/>
     </row>
@@ -2433,7 +2436,7 @@
         <v>87</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H58" s="8"/>
     </row>
@@ -2455,7 +2458,7 @@
         <v>87</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H59" s="8"/>
     </row>
@@ -2477,7 +2480,7 @@
         <v>87</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H60" s="8"/>
     </row>
@@ -2499,7 +2502,7 @@
         <v>87</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H61" s="8"/>
     </row>
@@ -2519,7 +2522,7 @@
         <v>84</v>
       </c>
       <c r="G62" s="15" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H62" s="16"/>
     </row>

</xml_diff>